<commit_message>
feat: implement dashboard page including a new header component and Excel export utility.
</commit_message>
<xml_diff>
--- a/public/dashboard_template.xlsx
+++ b/public/dashboard_template.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="29426"/>
   <workbookPr filterPrivacy="1" hidePivotFieldList="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{785930F4-DED2-46E0-8311-F560B9B4AF2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CA4F703-B3A6-4789-833F-FFFE1399D810}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="1" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Resumen Ejecutivo" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
   </sheets>
   <calcPr calcId="171027"/>
   <pivotCaches>
-    <pivotCache cacheId="20" r:id="rId7"/>
+    <pivotCache cacheId="0" r:id="rId7"/>
   </pivotCaches>
 </workbook>
 </file>
@@ -2023,7 +2023,7 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:pivotSource>
-    <c:name>[Dashboard_Report_2025-12-27 (4).xlsx]Volatilidad!TablaDinámica13</c:name>
+    <c:name>[dashboard_template.xlsx]Volatilidad!TablaDinámica13</c:name>
     <c:fmtId val="0"/>
   </c:pivotSource>
   <c:chart>
@@ -2041,19 +2041,7 @@
           <a:effectLst/>
         </c:spPr>
         <c:marker>
-          <c:symbol val="circle"/>
-          <c:size val="5"/>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent1"/>
-            </a:solidFill>
-            <a:ln w="9525">
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
+          <c:symbol val="none"/>
         </c:marker>
         <c:dLbl>
           <c:idx val="0"/>
@@ -5846,7 +5834,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{ADB6A451-3B0E-462C-8A22-13A1E714B737}" name="TablaDinámica13" cacheId="20" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" compactData="0" multipleFieldFilters="0" chartFormat="7">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{ADB6A451-3B0E-462C-8A22-13A1E714B737}" name="TablaDinámica13" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" compactData="0" multipleFieldFilters="0" chartFormat="7">
   <location ref="A3:C28" firstHeaderRow="1" firstDataRow="1" firstDataCol="2"/>
   <pivotFields count="3">
     <pivotField axis="axisRow" compact="0" outline="0" showAll="0" defaultSubtotal="0">
@@ -6431,9 +6419,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G28" sqref="G28"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -6577,7 +6563,7 @@
   <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="R19" sqref="R19"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7239,8 +7225,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6953E53E-7997-4BF1-AF5B-AE7E79E99135}">
   <dimension ref="A3:C28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="W27" sqref="W27"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>